<commit_message>
fix 滞納金一覧 Signed-off-by: LiuYiyang <lyy@shequchina.cn>
</commit_message>
<xml_diff>
--- a/test_請求管理/已完成/test_請求管理_滞納金一覧.xlsx
+++ b/test_請求管理/已完成/test_請求管理_滞納金一覧.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="27765" windowHeight="13650" tabRatio="758" activeTab="3"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="27765" windowHeight="13650" tabRatio="758" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="7" r:id="rId1"/>
@@ -16466,7 +16466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -16720,8 +16720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:BY54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I29" activeCellId="1" sqref="H52 I29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -16789,16 +16789,16 @@
       <c r="B5" s="9" t="s">
         <v>806</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>807</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>808</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>810</v>
       </c>
     </row>

</xml_diff>